<commit_message>
new plateplan and table
</commit_message>
<xml_diff>
--- a/template-pplan.xlsx
+++ b/template-pplan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Shef_covid\elisa-dl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B67B90F0-3DB6-4F1E-8F08-8EFBA0E0BF8A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{383648ED-33C8-426B-A064-C7D3E1477626}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="62">
   <si>
     <t xml:space="preserve"> A</t>
   </si>
@@ -65,126 +65,6 @@
     <t>BLK</t>
   </si>
   <si>
-    <t>sample10-dilution</t>
-  </si>
-  <si>
-    <t>sample11-dilution</t>
-  </si>
-  <si>
-    <t>sample12-dilution</t>
-  </si>
-  <si>
-    <t>sample13-dilution</t>
-  </si>
-  <si>
-    <t>sample14-dilution</t>
-  </si>
-  <si>
-    <t>sample15-dilution</t>
-  </si>
-  <si>
-    <t>sample16-dilution</t>
-  </si>
-  <si>
-    <t>sample17-dilution</t>
-  </si>
-  <si>
-    <t>sample18-dilution</t>
-  </si>
-  <si>
-    <t>sample19-dilution</t>
-  </si>
-  <si>
-    <t>sample20-dilution</t>
-  </si>
-  <si>
-    <t>sample01-dilution</t>
-  </si>
-  <si>
-    <t>sample01</t>
-  </si>
-  <si>
-    <t>sample02-dilution</t>
-  </si>
-  <si>
-    <t>sample03-dilution</t>
-  </si>
-  <si>
-    <t>sample04-dilution</t>
-  </si>
-  <si>
-    <t>sample05-dilution</t>
-  </si>
-  <si>
-    <t>sample06-dilution</t>
-  </si>
-  <si>
-    <t>sample07-dilution</t>
-  </si>
-  <si>
-    <t>sample08-dilution</t>
-  </si>
-  <si>
-    <t>sample09-dilution</t>
-  </si>
-  <si>
-    <t>sample02</t>
-  </si>
-  <si>
-    <t>sample03</t>
-  </si>
-  <si>
-    <t>sample04</t>
-  </si>
-  <si>
-    <t>sample05</t>
-  </si>
-  <si>
-    <t>sample06</t>
-  </si>
-  <si>
-    <t>sample07</t>
-  </si>
-  <si>
-    <t>sample08</t>
-  </si>
-  <si>
-    <t>sample09</t>
-  </si>
-  <si>
-    <t>sample10</t>
-  </si>
-  <si>
-    <t>sample11</t>
-  </si>
-  <si>
-    <t>sample12</t>
-  </si>
-  <si>
-    <t>sample13</t>
-  </si>
-  <si>
-    <t>sample14</t>
-  </si>
-  <si>
-    <t>sample15</t>
-  </si>
-  <si>
-    <t>sample16</t>
-  </si>
-  <si>
-    <t>sample17</t>
-  </si>
-  <si>
-    <t>sample18</t>
-  </si>
-  <si>
-    <t>sample19</t>
-  </si>
-  <si>
-    <t>sample20</t>
-  </si>
-  <si>
     <t>STD-1</t>
   </si>
   <si>
@@ -224,9 +104,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>sample21-dilution</t>
-  </si>
-  <si>
     <t>*Enter in the format sampleID-dilition. You just need to enter the first cell for each sample (the white boxes)</t>
   </si>
   <si>
@@ -242,14 +119,113 @@
     <t>*If the plate isn't full put EMPTY in place of the empty sampleID-barcode</t>
   </si>
   <si>
-    <t>sample21</t>
+    <t>S1-dilution</t>
+  </si>
+  <si>
+    <t>S2-dilution</t>
+  </si>
+  <si>
+    <t>S3-dilution</t>
+  </si>
+  <si>
+    <t>S4-dilution</t>
+  </si>
+  <si>
+    <t>S5-dilution</t>
+  </si>
+  <si>
+    <t>S6-dilution</t>
+  </si>
+  <si>
+    <t>S7-dilution</t>
+  </si>
+  <si>
+    <t>S8-dilution</t>
+  </si>
+  <si>
+    <t>S9-dilution</t>
+  </si>
+  <si>
+    <t>S10-dilution</t>
+  </si>
+  <si>
+    <t>S11-dilution</t>
+  </si>
+  <si>
+    <t>S12-dilution</t>
+  </si>
+  <si>
+    <t>S13-dilution</t>
+  </si>
+  <si>
+    <t>S14-dilution</t>
+  </si>
+  <si>
+    <t>S15-dilution</t>
+  </si>
+  <si>
+    <t>S16-dilution</t>
+  </si>
+  <si>
+    <t>S17-dilution</t>
+  </si>
+  <si>
+    <t>S18-dilution</t>
+  </si>
+  <si>
+    <t>S19-dilution</t>
+  </si>
+  <si>
+    <t>S20-dilution</t>
+  </si>
+  <si>
+    <t>S21-dilution</t>
+  </si>
+  <si>
+    <t>S22-dilution</t>
+  </si>
+  <si>
+    <t>S23-dilution</t>
+  </si>
+  <si>
+    <t>S24-dilution</t>
+  </si>
+  <si>
+    <t>S25-dilution</t>
+  </si>
+  <si>
+    <t>S26-dilution</t>
+  </si>
+  <si>
+    <t>S27-dilution</t>
+  </si>
+  <si>
+    <t>S28-dilution</t>
+  </si>
+  <si>
+    <t>29-dilution</t>
+  </si>
+  <si>
+    <t>S29-dilution</t>
+  </si>
+  <si>
+    <t>S30-dilution</t>
+  </si>
+  <si>
+    <t>S31-dilution</t>
+  </si>
+  <si>
+    <t>S32-dilution</t>
+  </si>
+  <si>
+    <t>NEG</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -265,8 +241,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -294,6 +276,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -338,7 +326,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -363,6 +351,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -648,49 +642,44 @@
   <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="X45" sqref="X45"/>
+      <selection activeCell="L40" sqref="L40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="9" width="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" customWidth="1"/>
+    <col min="11" max="13" width="13" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
-        <v>62</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>64</v>
+        <v>23</v>
       </c>
       <c r="J2" t="s">
-        <v>68</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>65</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>66</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>67</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -736,236 +725,236 @@
         <v>0</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>22</v>
+        <v>28</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>42</v>
+        <v>29</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="L7" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="M7" s="6" t="s">
-        <v>48</v>
+        <v>32</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" s="6" t="s">
+      <c r="B8" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="H8" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="I8" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="J8" s="6" t="s">
-        <v>43</v>
+      <c r="J8" s="10" t="s">
+        <v>38</v>
       </c>
       <c r="K8" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="L8" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="M8" s="6" t="s">
-        <v>49</v>
+        <v>38</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I9" s="6" t="s">
+      <c r="B9" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="J9" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J9" s="6" t="s">
+      <c r="K9" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="K9" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="L9" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="M9" s="6" t="s">
-        <v>69</v>
+      <c r="L9" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="J10" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="K10" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="L10" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="M10" s="5" t="s">
-        <v>8</v>
+      <c r="B10" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="J10" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I11" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="J11" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="K11" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="L11" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="M11" s="4" t="s">
-        <v>9</v>
+      <c r="B11" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="I11" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="J11" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I12" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="J12" s="6" t="s">
-        <v>47</v>
+      <c r="B12" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>9</v>
       </c>
       <c r="K12" s="9" t="s">
         <v>9</v>
@@ -982,40 +971,40 @@
         <v>6</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>53</v>
+        <v>13</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>56</v>
+        <v>16</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>57</v>
+        <v>17</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>59</v>
+        <v>19</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>61</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -1023,40 +1012,40 @@
         <v>7</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>53</v>
+        <v>13</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>56</v>
+        <v>16</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>57</v>
+        <v>17</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>59</v>
+        <v>19</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>61</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -1103,15 +1092,15 @@
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="6"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="2"/>
       <c r="G17" s="6"/>
       <c r="H17" s="2"/>
       <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="6"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="2"/>
       <c r="M17" s="6"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -1120,15 +1109,15 @@
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="6"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="2"/>
       <c r="G18" s="6"/>
       <c r="H18" s="2"/>
       <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="6"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="2"/>
       <c r="M18" s="6"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -1137,15 +1126,15 @@
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="6"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="2"/>
       <c r="G19" s="6"/>
       <c r="H19" s="2"/>
       <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="6"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="2"/>
       <c r="M19" s="6"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -1154,22 +1143,16 @@
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="6"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="2"/>
       <c r="G20" s="6"/>
       <c r="H20" s="2"/>
       <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="L20" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="M20" s="5" t="s">
-        <v>8</v>
-      </c>
+      <c r="J20" s="2"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="6"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
@@ -1177,22 +1160,16 @@
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="6"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="2"/>
       <c r="G21" s="6"/>
       <c r="H21" s="2"/>
       <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="L21" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="M21" s="4" t="s">
-        <v>9</v>
-      </c>
+      <c r="J21" s="2"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="6"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
@@ -1200,14 +1177,24 @@
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
-      <c r="K22" s="4" t="s">
+      <c r="D22" s="2"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H22" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="I22" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="J22" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="K22" s="9" t="s">
         <v>9</v>
       </c>
       <c r="L22" s="4" t="s">
@@ -1222,40 +1209,40 @@
         <v>6</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>53</v>
+        <v>13</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>56</v>
+        <v>16</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>57</v>
+        <v>17</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>59</v>
+        <v>19</v>
       </c>
       <c r="L23" s="3" t="s">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="M23" s="3" t="s">
-        <v>61</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
@@ -1263,40 +1250,40 @@
         <v>7</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>53</v>
+        <v>13</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>56</v>
+        <v>16</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>57</v>
+        <v>17</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>59</v>
+        <v>19</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="M24" s="3" t="s">
-        <v>61</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>